<commit_message>
ajout des utilisateurs et des menu principaux
</commit_message>
<xml_diff>
--- a/Doc/Journal de travail/journal_de_travail_Bataille_navale.xlsx
+++ b/Doc/Journal de travail/journal_de_travail_Bataille_navale.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sébastien Moraz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Battaille navale\Bataille_Navale 1.0\Doc\Journal de travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9757CED-A893-4681-8CAF-E1D0845C92A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2729BCC-DFEE-4E1B-82F3-EC8C2B8BCD73}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>Ajout des commentaire</t>
+  </si>
+  <si>
+    <t>Ajout de Menu principal + ajout des cartes aleatoire + ajout de fichier MCD</t>
   </si>
 </sst>
 </file>
@@ -788,7 +791,7 @@
   <dimension ref="A1:F673"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,12 +1064,24 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="14"/>
+      <c r="A14" s="8">
+        <v>43909</v>
+      </c>
+      <c r="B14" s="14">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
@@ -4680,7 +4695,7 @@
       </c>
       <c r="B1" s="17">
         <f>SUM(Journal!D2:D18)</f>
-        <v>0.72916666666666663</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>